<commit_message>
Update Create new curriculum class if no class found while import
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_NganhTatCa.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_NganhTatCa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08A1810-428E-4134-BA24-0B9177710294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34235C-CA43-45FF-978D-638E17C89A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6116" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6141" uniqueCount="682">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -3945,14 +3945,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PHÂNCÔNGHK222" displayName="PHÂNCÔNGHK222" ref="A1:AD226" totalsRowShown="0">
-  <autoFilter ref="A1:AD226" xr:uid="{00000000-0009-0000-0100-000001000000}">
-    <filterColumn colId="16">
-      <filters>
-        <filter val="Nguyễn Thị Diễm Anh"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PHÂNCÔNGHK222" displayName="PHÂNCÔNGHK222" ref="A1:AD227" totalsRowShown="0">
+  <autoFilter ref="A1:AD227" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MaGocLHP"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mã MH"/>
@@ -4274,10 +4268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD226"/>
+  <dimension ref="A1:AD227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q228" sqref="Q228"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="C229" sqref="C229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4382,7 +4376,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -4464,7 +4458,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -4546,7 +4540,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4628,7 +4622,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -4710,7 +4704,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -4793,7 +4787,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -4876,7 +4870,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -4959,7 +4953,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -5042,7 +5036,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -5125,7 +5119,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5208,7 +5202,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -5291,7 +5285,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -5374,7 +5368,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -5457,7 +5451,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -5540,7 +5534,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -5623,7 +5617,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -5706,7 +5700,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -5789,7 +5783,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -5872,7 +5866,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -5955,7 +5949,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -6038,7 +6032,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -6121,7 +6115,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -6204,7 +6198,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>153</v>
       </c>
@@ -6287,7 +6281,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -6370,7 +6364,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -6449,7 +6443,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -6528,7 +6522,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>164</v>
       </c>
@@ -6607,7 +6601,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -6690,7 +6684,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>172</v>
       </c>
@@ -6939,7 +6933,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -7022,7 +7016,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>190</v>
       </c>
@@ -7105,7 +7099,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -7188,7 +7182,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>202</v>
       </c>
@@ -7267,7 +7261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>208</v>
       </c>
@@ -7346,7 +7340,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>213</v>
       </c>
@@ -7425,7 +7419,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>215</v>
       </c>
@@ -7504,7 +7498,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>218</v>
       </c>
@@ -7586,7 +7580,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>223</v>
       </c>
@@ -7668,7 +7662,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -7750,7 +7744,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>229</v>
       </c>
@@ -7832,7 +7826,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -7918,7 +7912,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -8004,7 +7998,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -8090,7 +8084,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -8176,7 +8170,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -8262,7 +8256,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>264</v>
       </c>
@@ -8348,7 +8342,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>268</v>
       </c>
@@ -8431,7 +8425,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>276</v>
       </c>
@@ -8514,7 +8508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>279</v>
       </c>
@@ -8597,7 +8591,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>282</v>
       </c>
@@ -8680,7 +8674,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>284</v>
       </c>
@@ -8763,7 +8757,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>286</v>
       </c>
@@ -8846,7 +8840,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>289</v>
       </c>
@@ -8929,7 +8923,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -9012,7 +9006,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>293</v>
       </c>
@@ -9095,7 +9089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>295</v>
       </c>
@@ -9178,7 +9172,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>297</v>
       </c>
@@ -9261,7 +9255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>301</v>
       </c>
@@ -9344,7 +9338,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -9427,7 +9421,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>305</v>
       </c>
@@ -9510,7 +9504,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>307</v>
       </c>
@@ -9593,7 +9587,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>312</v>
       </c>
@@ -9676,7 +9670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>316</v>
       </c>
@@ -9759,7 +9753,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>318</v>
       </c>
@@ -9842,7 +9836,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>322</v>
       </c>
@@ -9925,7 +9919,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>325</v>
       </c>
@@ -10008,7 +10002,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>330</v>
       </c>
@@ -10087,7 +10081,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>332</v>
       </c>
@@ -10170,7 +10164,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>334</v>
       </c>
@@ -10253,7 +10247,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>343</v>
       </c>
@@ -10336,7 +10330,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>346</v>
       </c>
@@ -10419,7 +10413,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>348</v>
       </c>
@@ -10502,7 +10496,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>352</v>
       </c>
@@ -10588,7 +10582,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>358</v>
       </c>
@@ -10674,7 +10668,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>362</v>
       </c>
@@ -10760,7 +10754,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>364</v>
       </c>
@@ -10846,7 +10840,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>366</v>
       </c>
@@ -10929,7 +10923,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>366</v>
       </c>
@@ -11012,7 +11006,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>372</v>
       </c>
@@ -11095,7 +11089,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>372</v>
       </c>
@@ -11178,7 +11172,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>374</v>
       </c>
@@ -11261,7 +11255,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>374</v>
       </c>
@@ -11344,7 +11338,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>380</v>
       </c>
@@ -11427,7 +11421,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>380</v>
       </c>
@@ -11510,7 +11504,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>384</v>
       </c>
@@ -11593,7 +11587,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>394</v>
       </c>
@@ -11676,7 +11670,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>398</v>
       </c>
@@ -11759,7 +11753,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>399</v>
       </c>
@@ -11842,7 +11836,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>400</v>
       </c>
@@ -11925,7 +11919,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>401</v>
       </c>
@@ -12008,7 +12002,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>402</v>
       </c>
@@ -12091,7 +12085,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>403</v>
       </c>
@@ -12174,7 +12168,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>404</v>
       </c>
@@ -12257,7 +12251,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>405</v>
       </c>
@@ -12340,7 +12334,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>406</v>
       </c>
@@ -12506,7 +12500,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>410</v>
       </c>
@@ -12589,7 +12583,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>411</v>
       </c>
@@ -12672,7 +12666,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>412</v>
       </c>
@@ -12755,7 +12749,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>413</v>
       </c>
@@ -12838,7 +12832,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>414</v>
       </c>
@@ -13004,7 +12998,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>416</v>
       </c>
@@ -13087,7 +13081,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="107" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>417</v>
       </c>
@@ -13170,7 +13164,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>421</v>
       </c>
@@ -13253,7 +13247,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>423</v>
       </c>
@@ -13419,7 +13413,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>425</v>
       </c>
@@ -13502,7 +13496,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>428</v>
       </c>
@@ -13585,7 +13579,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>429</v>
       </c>
@@ -13668,7 +13662,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>430</v>
       </c>
@@ -13834,7 +13828,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>432</v>
       </c>
@@ -13917,7 +13911,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>433</v>
       </c>
@@ -14000,7 +13994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>434</v>
       </c>
@@ -14083,7 +14077,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>435</v>
       </c>
@@ -14166,7 +14160,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>436</v>
       </c>
@@ -14249,7 +14243,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>437</v>
       </c>
@@ -14332,7 +14326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>438</v>
       </c>
@@ -14415,7 +14409,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>441</v>
       </c>
@@ -14498,7 +14492,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>442</v>
       </c>
@@ -14581,7 +14575,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>448</v>
       </c>
@@ -14664,7 +14658,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>450</v>
       </c>
@@ -14747,7 +14741,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>452</v>
       </c>
@@ -14830,7 +14824,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>454</v>
       </c>
@@ -14916,7 +14910,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>456</v>
       </c>
@@ -15002,7 +14996,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>459</v>
       </c>
@@ -15088,7 +15082,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>461</v>
       </c>
@@ -15174,7 +15168,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>463</v>
       </c>
@@ -15257,7 +15251,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>468</v>
       </c>
@@ -15340,7 +15334,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>469</v>
       </c>
@@ -15423,7 +15417,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>470</v>
       </c>
@@ -15506,7 +15500,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>473</v>
       </c>
@@ -15589,7 +15583,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>474</v>
       </c>
@@ -15672,7 +15666,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>477</v>
       </c>
@@ -15755,7 +15749,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>478</v>
       </c>
@@ -15838,7 +15832,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>481</v>
       </c>
@@ -15921,7 +15915,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>483</v>
       </c>
@@ -16004,7 +15998,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>484</v>
       </c>
@@ -16087,7 +16081,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>485</v>
       </c>
@@ -16170,7 +16164,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>488</v>
       </c>
@@ -16253,7 +16247,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="145" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>489</v>
       </c>
@@ -16336,7 +16330,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="146" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>490</v>
       </c>
@@ -16419,7 +16413,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="147" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>491</v>
       </c>
@@ -16502,7 +16496,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="148" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>492</v>
       </c>
@@ -16585,7 +16579,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="149" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>493</v>
       </c>
@@ -16668,7 +16662,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="150" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>494</v>
       </c>
@@ -16751,7 +16745,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>497</v>
       </c>
@@ -16834,7 +16828,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="152" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>498</v>
       </c>
@@ -16917,7 +16911,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="153" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>500</v>
       </c>
@@ -17000,7 +16994,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="154" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>501</v>
       </c>
@@ -17083,7 +17077,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>502</v>
       </c>
@@ -17166,7 +17160,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>503</v>
       </c>
@@ -17249,7 +17243,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="157" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>504</v>
       </c>
@@ -17332,7 +17326,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>505</v>
       </c>
@@ -17415,7 +17409,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="159" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>506</v>
       </c>
@@ -17498,7 +17492,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>507</v>
       </c>
@@ -17581,7 +17575,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>508</v>
       </c>
@@ -17664,7 +17658,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>509</v>
       </c>
@@ -17747,7 +17741,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>512</v>
       </c>
@@ -17830,7 +17824,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>513</v>
       </c>
@@ -17913,7 +17907,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>514</v>
       </c>
@@ -17996,7 +17990,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>517</v>
       </c>
@@ -18079,7 +18073,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>518</v>
       </c>
@@ -18162,7 +18156,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>519</v>
       </c>
@@ -18245,7 +18239,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>525</v>
       </c>
@@ -18328,7 +18322,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>529</v>
       </c>
@@ -18411,7 +18405,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>531</v>
       </c>
@@ -18494,7 +18488,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>533</v>
       </c>
@@ -18577,7 +18571,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>535</v>
       </c>
@@ -18663,7 +18657,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>540</v>
       </c>
@@ -18749,7 +18743,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>543</v>
       </c>
@@ -18835,7 +18829,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>546</v>
       </c>
@@ -18921,7 +18915,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>548</v>
       </c>
@@ -19007,7 +19001,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>550</v>
       </c>
@@ -19093,7 +19087,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>553</v>
       </c>
@@ -19179,7 +19173,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>557</v>
       </c>
@@ -19265,7 +19259,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>559</v>
       </c>
@@ -19348,7 +19342,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="182" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>566</v>
       </c>
@@ -19431,7 +19425,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="183" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>568</v>
       </c>
@@ -19514,7 +19508,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>570</v>
       </c>
@@ -19597,7 +19591,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>572</v>
       </c>
@@ -19680,7 +19674,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>575</v>
       </c>
@@ -19763,7 +19757,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>577</v>
       </c>
@@ -19846,7 +19840,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>579</v>
       </c>
@@ -19929,7 +19923,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>582</v>
       </c>
@@ -20012,7 +20006,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>586</v>
       </c>
@@ -20095,7 +20089,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>590</v>
       </c>
@@ -20178,7 +20172,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="192" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>592</v>
       </c>
@@ -20261,7 +20255,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>594</v>
       </c>
@@ -20347,7 +20341,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>597</v>
       </c>
@@ -20433,7 +20427,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>599</v>
       </c>
@@ -20519,7 +20513,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>601</v>
       </c>
@@ -20605,7 +20599,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="197" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>603</v>
       </c>
@@ -20691,7 +20685,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>605</v>
       </c>
@@ -20777,7 +20771,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>608</v>
       </c>
@@ -20863,7 +20857,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="200" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>611</v>
       </c>
@@ -20949,7 +20943,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="201" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>613</v>
       </c>
@@ -21035,7 +21029,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="202" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>615</v>
       </c>
@@ -21121,7 +21115,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="203" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>617</v>
       </c>
@@ -21204,7 +21198,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="204" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>621</v>
       </c>
@@ -21287,7 +21281,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="205" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>625</v>
       </c>
@@ -21370,7 +21364,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>627</v>
       </c>
@@ -21453,7 +21447,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>629</v>
       </c>
@@ -21539,7 +21533,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>632</v>
       </c>
@@ -21625,7 +21619,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>634</v>
       </c>
@@ -21711,7 +21705,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>636</v>
       </c>
@@ -21797,7 +21791,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>640</v>
       </c>
@@ -21883,7 +21877,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>642</v>
       </c>
@@ -21969,7 +21963,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>645</v>
       </c>
@@ -22055,7 +22049,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>648</v>
       </c>
@@ -22138,7 +22132,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="215" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>655</v>
       </c>
@@ -22221,7 +22215,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="216" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>657</v>
       </c>
@@ -22304,7 +22298,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="217" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>659</v>
       </c>
@@ -22387,7 +22381,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>661</v>
       </c>
@@ -22470,7 +22464,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="219" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>664</v>
       </c>
@@ -22553,7 +22547,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="220" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>666</v>
       </c>
@@ -22636,7 +22630,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="221" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>668</v>
       </c>
@@ -22719,7 +22713,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="222" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>670</v>
       </c>
@@ -22805,7 +22799,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>670</v>
       </c>
@@ -22891,7 +22885,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>674</v>
       </c>
@@ -22965,7 +22959,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="225" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>674</v>
       </c>
@@ -23039,7 +23033,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="226" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>678</v>
       </c>
@@ -23119,6 +23113,89 @@
         <v>47</v>
       </c>
       <c r="AB226" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="227" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A227">
+        <v>123</v>
+      </c>
+      <c r="B227" t="s">
+        <v>678</v>
+      </c>
+      <c r="C227">
+        <v>123</v>
+      </c>
+      <c r="D227" t="s">
+        <v>680</v>
+      </c>
+      <c r="E227" t="s">
+        <v>33</v>
+      </c>
+      <c r="F227" t="s">
+        <v>34</v>
+      </c>
+      <c r="G227" t="s">
+        <v>681</v>
+      </c>
+      <c r="H227" t="s">
+        <v>36</v>
+      </c>
+      <c r="I227" t="s">
+        <v>37</v>
+      </c>
+      <c r="K227" t="s">
+        <v>64</v>
+      </c>
+      <c r="L227" t="s">
+        <v>167</v>
+      </c>
+      <c r="M227" t="s">
+        <v>33</v>
+      </c>
+      <c r="N227" t="s">
+        <v>168</v>
+      </c>
+      <c r="O227" t="s">
+        <v>143</v>
+      </c>
+      <c r="P227" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q227" t="s">
+        <v>93</v>
+      </c>
+      <c r="R227" t="s">
+        <v>42</v>
+      </c>
+      <c r="S227" t="s">
+        <v>43</v>
+      </c>
+      <c r="T227" t="s">
+        <v>43</v>
+      </c>
+      <c r="U227" t="s">
+        <v>44</v>
+      </c>
+      <c r="V227" t="s">
+        <v>45</v>
+      </c>
+      <c r="W227" t="s">
+        <v>46</v>
+      </c>
+      <c r="X227" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y227" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z227" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA227" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB227" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update  Refresh timetable when user is viewing all majors
</commit_message>
<xml_diff>
--- a/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_NganhTatCa.xlsx
+++ b/TeachingAssignmentManagement/Uploads/CNTT ThoiKhoaBieu_HK222_NganhTatCa.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\duy94\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34235C-CA43-45FF-978D-638E17C89A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E861525-1EC9-4808-B602-30D6119DC905}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6141" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6116" uniqueCount="682">
   <si>
     <t>MaGocLHP</t>
   </si>
@@ -3945,8 +3945,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PHÂNCÔNGHK222" displayName="PHÂNCÔNGHK222" ref="A1:AD227" totalsRowShown="0">
-  <autoFilter ref="A1:AD227" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="PHÂNCÔNGHK222" displayName="PHÂNCÔNGHK222" ref="A1:AD226" totalsRowShown="0">
+  <autoFilter ref="A1:AD226" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="16">
+      <filters>
+        <filter val="Nguyễn Thị Diễm Anh"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="30">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="MaGocLHP"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Mã MH"/>
@@ -4268,10 +4274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD227"/>
+  <dimension ref="A1:AD226"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
-      <selection activeCell="C229" sqref="C229"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="Q228" sqref="Q228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4376,7 +4382,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -4458,7 +4464,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -4540,7 +4546,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -4622,7 +4628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -4704,7 +4710,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -4787,7 +4793,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -4870,7 +4876,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>78</v>
       </c>
@@ -4953,7 +4959,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
@@ -5036,7 +5042,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -5119,7 +5125,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -5202,7 +5208,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>96</v>
       </c>
@@ -5285,7 +5291,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>96</v>
       </c>
@@ -5368,7 +5374,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>102</v>
       </c>
@@ -5451,7 +5457,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>102</v>
       </c>
@@ -5534,7 +5540,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>116</v>
       </c>
@@ -5617,7 +5623,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>116</v>
       </c>
@@ -5700,7 +5706,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -5783,7 +5789,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -5866,7 +5872,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -5949,7 +5955,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>137</v>
       </c>
@@ -6032,7 +6038,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>144</v>
       </c>
@@ -6115,7 +6121,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>144</v>
       </c>
@@ -6198,7 +6204,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>153</v>
       </c>
@@ -6281,7 +6287,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>153</v>
       </c>
@@ -6364,7 +6370,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>156</v>
       </c>
@@ -6443,7 +6449,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>156</v>
       </c>
@@ -6522,7 +6528,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>164</v>
       </c>
@@ -6601,7 +6607,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>172</v>
       </c>
@@ -6684,7 +6690,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>172</v>
       </c>
@@ -6933,7 +6939,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>183</v>
       </c>
@@ -7016,7 +7022,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>190</v>
       </c>
@@ -7099,7 +7105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -7182,7 +7188,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>202</v>
       </c>
@@ -7261,7 +7267,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>208</v>
       </c>
@@ -7340,7 +7346,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>213</v>
       </c>
@@ -7419,7 +7425,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>215</v>
       </c>
@@ -7498,7 +7504,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>218</v>
       </c>
@@ -7580,7 +7586,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>223</v>
       </c>
@@ -7662,7 +7668,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>226</v>
       </c>
@@ -7744,7 +7750,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>229</v>
       </c>
@@ -7826,7 +7832,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>232</v>
       </c>
@@ -7912,7 +7918,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>242</v>
       </c>
@@ -7998,7 +8004,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>248</v>
       </c>
@@ -8084,7 +8090,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>255</v>
       </c>
@@ -8170,7 +8176,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>258</v>
       </c>
@@ -8256,7 +8262,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>264</v>
       </c>
@@ -8342,7 +8348,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>268</v>
       </c>
@@ -8425,7 +8431,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>276</v>
       </c>
@@ -8508,7 +8514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>279</v>
       </c>
@@ -8591,7 +8597,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>282</v>
       </c>
@@ -8674,7 +8680,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>284</v>
       </c>
@@ -8757,7 +8763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>286</v>
       </c>
@@ -8840,7 +8846,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>289</v>
       </c>
@@ -8923,7 +8929,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>291</v>
       </c>
@@ -9006,7 +9012,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>293</v>
       </c>
@@ -9089,7 +9095,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>295</v>
       </c>
@@ -9172,7 +9178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>297</v>
       </c>
@@ -9255,7 +9261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>301</v>
       </c>
@@ -9338,7 +9344,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>303</v>
       </c>
@@ -9421,7 +9427,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>305</v>
       </c>
@@ -9504,7 +9510,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>307</v>
       </c>
@@ -9587,7 +9593,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>312</v>
       </c>
@@ -9670,7 +9676,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>316</v>
       </c>
@@ -9753,7 +9759,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>318</v>
       </c>
@@ -9836,7 +9842,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>322</v>
       </c>
@@ -9919,7 +9925,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>325</v>
       </c>
@@ -10002,7 +10008,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>330</v>
       </c>
@@ -10081,7 +10087,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>332</v>
       </c>
@@ -10164,7 +10170,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>334</v>
       </c>
@@ -10247,7 +10253,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>343</v>
       </c>
@@ -10330,7 +10336,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>346</v>
       </c>
@@ -10413,7 +10419,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>348</v>
       </c>
@@ -10496,7 +10502,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>352</v>
       </c>
@@ -10582,7 +10588,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>358</v>
       </c>
@@ -10668,7 +10674,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>362</v>
       </c>
@@ -10754,7 +10760,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>364</v>
       </c>
@@ -10840,7 +10846,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>366</v>
       </c>
@@ -10923,7 +10929,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="81" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>366</v>
       </c>
@@ -11006,7 +11012,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="82" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>372</v>
       </c>
@@ -11089,7 +11095,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="83" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>372</v>
       </c>
@@ -11172,7 +11178,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>374</v>
       </c>
@@ -11255,7 +11261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="85" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>374</v>
       </c>
@@ -11338,7 +11344,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="86" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>380</v>
       </c>
@@ -11421,7 +11427,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="87" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>380</v>
       </c>
@@ -11504,7 +11510,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="88" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>384</v>
       </c>
@@ -11587,7 +11593,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="89" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>394</v>
       </c>
@@ -11670,7 +11676,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>398</v>
       </c>
@@ -11753,7 +11759,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>399</v>
       </c>
@@ -11836,7 +11842,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>400</v>
       </c>
@@ -11919,7 +11925,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="93" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>401</v>
       </c>
@@ -12002,7 +12008,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>402</v>
       </c>
@@ -12085,7 +12091,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>403</v>
       </c>
@@ -12168,7 +12174,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>404</v>
       </c>
@@ -12251,7 +12257,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="97" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>405</v>
       </c>
@@ -12334,7 +12340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>406</v>
       </c>
@@ -12500,7 +12506,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>410</v>
       </c>
@@ -12583,7 +12589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="101" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>411</v>
       </c>
@@ -12666,7 +12672,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>412</v>
       </c>
@@ -12749,7 +12755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>413</v>
       </c>
@@ -12832,7 +12838,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>414</v>
       </c>
@@ -12998,7 +13004,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>416</v>
       </c>
@@ -13081,7 +13087,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="107" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>417</v>
       </c>
@@ -13164,7 +13170,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>421</v>
       </c>
@@ -13247,7 +13253,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="109" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>423</v>
       </c>
@@ -13413,7 +13419,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>425</v>
       </c>
@@ -13496,7 +13502,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>428</v>
       </c>
@@ -13579,7 +13585,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>429</v>
       </c>
@@ -13662,7 +13668,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>430</v>
       </c>
@@ -13828,7 +13834,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>432</v>
       </c>
@@ -13911,7 +13917,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>433</v>
       </c>
@@ -13994,7 +14000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>434</v>
       </c>
@@ -14077,7 +14083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>435</v>
       </c>
@@ -14160,7 +14166,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>436</v>
       </c>
@@ -14243,7 +14249,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>437</v>
       </c>
@@ -14326,7 +14332,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>438</v>
       </c>
@@ -14409,7 +14415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>441</v>
       </c>
@@ -14492,7 +14498,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>442</v>
       </c>
@@ -14575,7 +14581,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>448</v>
       </c>
@@ -14658,7 +14664,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>450</v>
       </c>
@@ -14741,7 +14747,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>452</v>
       </c>
@@ -14824,7 +14830,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>454</v>
       </c>
@@ -14910,7 +14916,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>456</v>
       </c>
@@ -14996,7 +15002,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>459</v>
       </c>
@@ -15082,7 +15088,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>461</v>
       </c>
@@ -15168,7 +15174,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>463</v>
       </c>
@@ -15251,7 +15257,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>468</v>
       </c>
@@ -15334,7 +15340,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>469</v>
       </c>
@@ -15417,7 +15423,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>470</v>
       </c>
@@ -15500,7 +15506,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>473</v>
       </c>
@@ -15583,7 +15589,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>474</v>
       </c>
@@ -15666,7 +15672,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>477</v>
       </c>
@@ -15749,7 +15755,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>478</v>
       </c>
@@ -15832,7 +15838,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>481</v>
       </c>
@@ -15915,7 +15921,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>483</v>
       </c>
@@ -15998,7 +16004,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>484</v>
       </c>
@@ -16081,7 +16087,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>485</v>
       </c>
@@ -16164,7 +16170,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>488</v>
       </c>
@@ -16247,7 +16253,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="145" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>489</v>
       </c>
@@ -16330,7 +16336,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="146" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>490</v>
       </c>
@@ -16413,7 +16419,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="147" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>491</v>
       </c>
@@ -16496,7 +16502,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="148" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>492</v>
       </c>
@@ -16579,7 +16585,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="149" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>493</v>
       </c>
@@ -16662,7 +16668,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="150" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>494</v>
       </c>
@@ -16745,7 +16751,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="151" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>497</v>
       </c>
@@ -16828,7 +16834,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="152" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>498</v>
       </c>
@@ -16911,7 +16917,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="153" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>500</v>
       </c>
@@ -16994,7 +17000,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="154" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>501</v>
       </c>
@@ -17077,7 +17083,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="155" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>502</v>
       </c>
@@ -17160,7 +17166,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="156" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>503</v>
       </c>
@@ -17243,7 +17249,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="157" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>504</v>
       </c>
@@ -17326,7 +17332,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="158" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>505</v>
       </c>
@@ -17409,7 +17415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="159" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>506</v>
       </c>
@@ -17492,7 +17498,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="160" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>507</v>
       </c>
@@ -17575,7 +17581,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>508</v>
       </c>
@@ -17658,7 +17664,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>509</v>
       </c>
@@ -17741,7 +17747,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>512</v>
       </c>
@@ -17824,7 +17830,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>513</v>
       </c>
@@ -17907,7 +17913,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>514</v>
       </c>
@@ -17990,7 +17996,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>517</v>
       </c>
@@ -18073,7 +18079,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>518</v>
       </c>
@@ -18156,7 +18162,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>519</v>
       </c>
@@ -18239,7 +18245,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>525</v>
       </c>
@@ -18322,7 +18328,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>529</v>
       </c>
@@ -18405,7 +18411,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>531</v>
       </c>
@@ -18488,7 +18494,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>533</v>
       </c>
@@ -18571,7 +18577,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>535</v>
       </c>
@@ -18657,7 +18663,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>540</v>
       </c>
@@ -18743,7 +18749,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="175" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>543</v>
       </c>
@@ -18829,7 +18835,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="176" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>546</v>
       </c>
@@ -18915,7 +18921,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="177" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>548</v>
       </c>
@@ -19001,7 +19007,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="178" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>550</v>
       </c>
@@ -19087,7 +19093,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="179" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>553</v>
       </c>
@@ -19173,7 +19179,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="180" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>557</v>
       </c>
@@ -19259,7 +19265,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="181" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>559</v>
       </c>
@@ -19342,7 +19348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="182" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>566</v>
       </c>
@@ -19425,7 +19431,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="183" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>568</v>
       </c>
@@ -19508,7 +19514,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="184" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>570</v>
       </c>
@@ -19591,7 +19597,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="185" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>572</v>
       </c>
@@ -19674,7 +19680,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="186" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>575</v>
       </c>
@@ -19757,7 +19763,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="187" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>577</v>
       </c>
@@ -19840,7 +19846,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="188" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>579</v>
       </c>
@@ -19923,7 +19929,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="189" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>582</v>
       </c>
@@ -20006,7 +20012,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="190" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>586</v>
       </c>
@@ -20089,7 +20095,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="191" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>590</v>
       </c>
@@ -20172,7 +20178,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="192" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>592</v>
       </c>
@@ -20255,7 +20261,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="193" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>594</v>
       </c>
@@ -20341,7 +20347,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="194" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>597</v>
       </c>
@@ -20427,7 +20433,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="195" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>599</v>
       </c>
@@ -20513,7 +20519,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="196" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>601</v>
       </c>
@@ -20599,7 +20605,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="197" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>603</v>
       </c>
@@ -20685,7 +20691,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="198" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>605</v>
       </c>
@@ -20771,7 +20777,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="199" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>608</v>
       </c>
@@ -20857,7 +20863,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="200" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>611</v>
       </c>
@@ -20943,7 +20949,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="201" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>613</v>
       </c>
@@ -21029,7 +21035,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="202" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>615</v>
       </c>
@@ -21115,7 +21121,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="203" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>617</v>
       </c>
@@ -21198,7 +21204,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="204" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>621</v>
       </c>
@@ -21281,7 +21287,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="205" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>625</v>
       </c>
@@ -21364,7 +21370,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="206" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>627</v>
       </c>
@@ -21447,7 +21453,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="207" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>629</v>
       </c>
@@ -21533,7 +21539,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="208" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>632</v>
       </c>
@@ -21619,7 +21625,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="209" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>634</v>
       </c>
@@ -21705,7 +21711,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="210" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>636</v>
       </c>
@@ -21791,7 +21797,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="211" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>640</v>
       </c>
@@ -21877,7 +21883,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="212" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>642</v>
       </c>
@@ -21963,7 +21969,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="213" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>645</v>
       </c>
@@ -22049,7 +22055,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="214" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>648</v>
       </c>
@@ -22132,7 +22138,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="215" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>655</v>
       </c>
@@ -22215,7 +22221,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="216" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>657</v>
       </c>
@@ -22298,7 +22304,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="217" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>659</v>
       </c>
@@ -22381,7 +22387,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="218" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>661</v>
       </c>
@@ -22464,7 +22470,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="219" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>664</v>
       </c>
@@ -22547,7 +22553,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="220" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>666</v>
       </c>
@@ -22630,7 +22636,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="221" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>668</v>
       </c>
@@ -22713,7 +22719,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="222" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>670</v>
       </c>
@@ -22799,7 +22805,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="223" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>670</v>
       </c>
@@ -22885,7 +22891,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:29" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>674</v>
       </c>
@@ -22959,7 +22965,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="225" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>674</v>
       </c>
@@ -23033,7 +23039,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="226" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:28" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>678</v>
       </c>
@@ -23113,89 +23119,6 @@
         <v>47</v>
       </c>
       <c r="AB226" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="227" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A227">
-        <v>123</v>
-      </c>
-      <c r="B227" t="s">
-        <v>678</v>
-      </c>
-      <c r="C227">
-        <v>123</v>
-      </c>
-      <c r="D227" t="s">
-        <v>680</v>
-      </c>
-      <c r="E227" t="s">
-        <v>33</v>
-      </c>
-      <c r="F227" t="s">
-        <v>34</v>
-      </c>
-      <c r="G227" t="s">
-        <v>681</v>
-      </c>
-      <c r="H227" t="s">
-        <v>36</v>
-      </c>
-      <c r="I227" t="s">
-        <v>37</v>
-      </c>
-      <c r="K227" t="s">
-        <v>64</v>
-      </c>
-      <c r="L227" t="s">
-        <v>167</v>
-      </c>
-      <c r="M227" t="s">
-        <v>33</v>
-      </c>
-      <c r="N227" t="s">
-        <v>168</v>
-      </c>
-      <c r="O227" t="s">
-        <v>143</v>
-      </c>
-      <c r="P227" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q227" t="s">
-        <v>93</v>
-      </c>
-      <c r="R227" t="s">
-        <v>42</v>
-      </c>
-      <c r="S227" t="s">
-        <v>43</v>
-      </c>
-      <c r="T227" t="s">
-        <v>43</v>
-      </c>
-      <c r="U227" t="s">
-        <v>44</v>
-      </c>
-      <c r="V227" t="s">
-        <v>45</v>
-      </c>
-      <c r="W227" t="s">
-        <v>46</v>
-      </c>
-      <c r="X227" t="s">
-        <v>74</v>
-      </c>
-      <c r="Y227" t="s">
-        <v>167</v>
-      </c>
-      <c r="Z227" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA227" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB227" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>